<commit_message>
Update the example data.
</commit_message>
<xml_diff>
--- a/data/SampleData_PP2CAssay.xlsx
+++ b/data/SampleData_PP2CAssay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zenanxing/Documents/Exp_Data/TidyBuddy/Tidy-Buddy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C484EF1-71A5-A943-8938-258AFDBE43FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88604082-DD80-B545-88F0-7931648DD0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="1080" windowWidth="23320" windowHeight="17880" xr2:uid="{14DBDB46-EC3B-344E-A159-986F3E2C9D53}"/>
+    <workbookView xWindow="5440" yWindow="1080" windowWidth="23320" windowHeight="17880" activeTab="6" xr2:uid="{14DBDB46-EC3B-344E-A159-986F3E2C9D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Protein" sheetId="8" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Con_nM" sheetId="4" r:id="rId4"/>
     <sheet name="Replicate" sheetId="10" r:id="rId5"/>
     <sheet name="PP2C_Activity" sheetId="5" r:id="rId6"/>
+    <sheet name="Original_Data" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="18">
   <si>
     <t>B</t>
   </si>
@@ -83,6 +84,18 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>Replicate</t>
+  </si>
+  <si>
+    <t>Con_nM</t>
   </si>
 </sst>
 </file>
@@ -481,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3683CEC9-CC44-CE4A-8743-A9EFA3FC3176}">
   <dimension ref="A1:CS19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1834,7 +1847,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2662,7 +2675,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="B2" sqref="B2:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3044,4 +3057,424 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A00E5F-043E-C44D-B2B1-4E33972CBFC5}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B4" s="5">
+        <v>5.4378080000000004</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5.7129700000000003</v>
+      </c>
+      <c r="D4" s="5">
+        <v>6.1538830000000004</v>
+      </c>
+      <c r="E4" s="5">
+        <v>6.2571149999999998</v>
+      </c>
+      <c r="F4" s="5">
+        <v>8.0371240000000004</v>
+      </c>
+      <c r="G4" s="5">
+        <v>6.3505310000000001</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.74690500000000004</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3.8373159999999999</v>
+      </c>
+      <c r="J4" s="5">
+        <v>3.6045630000000002</v>
+      </c>
+      <c r="K4" s="5">
+        <v>2.0028009999999998</v>
+      </c>
+      <c r="L4" s="5">
+        <v>3.6759249999999999</v>
+      </c>
+      <c r="M4" s="5">
+        <v>3.6005989999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="5">
+        <v>10.96649</v>
+      </c>
+      <c r="C5" s="5">
+        <v>10.54702</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6.7885369999999998</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8.3268260000000005</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4.4356669999999996</v>
+      </c>
+      <c r="G5" s="5">
+        <v>6.4766620000000001</v>
+      </c>
+      <c r="H5" s="5">
+        <v>12.79105</v>
+      </c>
+      <c r="I5" s="5">
+        <v>11.029299999999999</v>
+      </c>
+      <c r="J5" s="5">
+        <v>10.5486</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1.0182709999999999</v>
+      </c>
+      <c r="L5" s="5">
+        <v>5.7940290000000001</v>
+      </c>
+      <c r="M5" s="5">
+        <v>4.842536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f t="shared" ref="A6:A10" si="0">A5/3</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="B6" s="5">
+        <v>31.875520000000002</v>
+      </c>
+      <c r="C6" s="5">
+        <v>32.046720000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>24.757660000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7.4529959999999997</v>
+      </c>
+      <c r="F6" s="5">
+        <v>6.2952810000000001</v>
+      </c>
+      <c r="G6" s="5">
+        <v>10.06467</v>
+      </c>
+      <c r="H6" s="5">
+        <v>19.1554</v>
+      </c>
+      <c r="I6" s="5">
+        <v>20.9221</v>
+      </c>
+      <c r="J6" s="5">
+        <v>21.753419999999998</v>
+      </c>
+      <c r="K6" s="5">
+        <v>6.913189</v>
+      </c>
+      <c r="L6" s="5">
+        <v>5.5144450000000003</v>
+      </c>
+      <c r="M6" s="5">
+        <v>9.2407120000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>111.1111111111111</v>
+      </c>
+      <c r="B7" s="5">
+        <v>65.006529999999998</v>
+      </c>
+      <c r="C7" s="5">
+        <v>63.774299999999997</v>
+      </c>
+      <c r="D7" s="5">
+        <v>51.448360000000001</v>
+      </c>
+      <c r="E7" s="5">
+        <v>17.10474</v>
+      </c>
+      <c r="F7" s="5">
+        <v>15.8278</v>
+      </c>
+      <c r="G7" s="5">
+        <v>19.26642</v>
+      </c>
+      <c r="H7" s="5">
+        <v>38.687019999999997</v>
+      </c>
+      <c r="I7" s="5">
+        <v>38.615160000000003</v>
+      </c>
+      <c r="J7" s="5">
+        <v>39.655439999999999</v>
+      </c>
+      <c r="K7" s="5">
+        <v>6.0091890000000001</v>
+      </c>
+      <c r="L7" s="5">
+        <v>5.7898990000000001</v>
+      </c>
+      <c r="M7" s="5">
+        <v>7.1634520000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>37.037037037037031</v>
+      </c>
+      <c r="B8" s="5">
+        <v>82.995639999999995</v>
+      </c>
+      <c r="C8" s="5">
+        <v>81.072779999999995</v>
+      </c>
+      <c r="D8" s="5">
+        <v>76.431010000000001</v>
+      </c>
+      <c r="E8" s="5">
+        <v>36.861510000000003</v>
+      </c>
+      <c r="F8" s="5">
+        <v>40.049309999999998</v>
+      </c>
+      <c r="G8" s="5">
+        <v>42.204810000000002</v>
+      </c>
+      <c r="H8" s="5">
+        <v>66.695350000000005</v>
+      </c>
+      <c r="I8" s="5">
+        <v>61.479480000000002</v>
+      </c>
+      <c r="J8" s="5">
+        <v>68.87585</v>
+      </c>
+      <c r="K8" s="5">
+        <v>18.893160000000002</v>
+      </c>
+      <c r="L8" s="5">
+        <v>19.058350000000001</v>
+      </c>
+      <c r="M8" s="5">
+        <v>24.164359999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>12.345679012345677</v>
+      </c>
+      <c r="B9" s="5">
+        <v>95.532409999999999</v>
+      </c>
+      <c r="C9" s="5">
+        <v>90.636200000000002</v>
+      </c>
+      <c r="D9" s="5">
+        <v>91.672139999999999</v>
+      </c>
+      <c r="E9" s="5">
+        <v>63.821550000000002</v>
+      </c>
+      <c r="F9" s="5">
+        <v>70.059039999999996</v>
+      </c>
+      <c r="G9" s="5">
+        <v>74.813479999999998</v>
+      </c>
+      <c r="H9" s="5">
+        <v>83.557090000000002</v>
+      </c>
+      <c r="I9" s="5">
+        <v>82.161230000000003</v>
+      </c>
+      <c r="J9" s="5">
+        <v>84.71754</v>
+      </c>
+      <c r="K9" s="5">
+        <v>52.204079999999998</v>
+      </c>
+      <c r="L9" s="5">
+        <v>55.813470000000002</v>
+      </c>
+      <c r="M9" s="5">
+        <v>58.75385</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1152263374485587</v>
+      </c>
+      <c r="B10" s="5">
+        <v>98.207689999999999</v>
+      </c>
+      <c r="C10" s="5">
+        <v>86.423349999999999</v>
+      </c>
+      <c r="D10" s="5">
+        <v>95.354299999999995</v>
+      </c>
+      <c r="E10" s="5">
+        <v>92.599040000000002</v>
+      </c>
+      <c r="F10" s="5">
+        <v>90.672550000000001</v>
+      </c>
+      <c r="G10" s="5">
+        <v>90.650739999999999</v>
+      </c>
+      <c r="H10" s="5">
+        <v>92.464939999999999</v>
+      </c>
+      <c r="I10" s="5">
+        <v>80.521720000000002</v>
+      </c>
+      <c r="J10" s="5">
+        <v>88.331069999999997</v>
+      </c>
+      <c r="K10" s="5">
+        <v>84.556479999999993</v>
+      </c>
+      <c r="L10" s="5">
+        <v>80.942959999999999</v>
+      </c>
+      <c r="M10" s="5">
+        <v>83.552959999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5">
+        <v>102.16249999999999</v>
+      </c>
+      <c r="C11" s="5">
+        <v>113.4924</v>
+      </c>
+      <c r="D11" s="5">
+        <v>86.48151</v>
+      </c>
+      <c r="E11" s="5">
+        <v>89.858329999999995</v>
+      </c>
+      <c r="F11" s="5">
+        <v>100.8139</v>
+      </c>
+      <c r="G11" s="5">
+        <v>93.031599999999997</v>
+      </c>
+      <c r="H11" s="5">
+        <v>99.241849999999999</v>
+      </c>
+      <c r="I11" s="5">
+        <v>97.792310000000001</v>
+      </c>
+      <c r="J11" s="5">
+        <v>100.0761</v>
+      </c>
+      <c r="K11" s="5">
+        <v>106.33669999999999</v>
+      </c>
+      <c r="L11" s="5">
+        <v>98.655420000000007</v>
+      </c>
+      <c r="M11" s="5">
+        <v>93.757549999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>